<commit_message>
Fixed lookup table. Some letters were not correctly matching. All letters are fine now. Now all I need to do is to extend it to account for tail-unioning
</commit_message>
<xml_diff>
--- a/misc/lookup_table.xlsx
+++ b/misc/lookup_table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksidac/Documents/Programming/Undertale/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D60064-BCD6-E44E-9BED-57D839C906A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1201E0-3366-FA49-BA47-8FBA16CB87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -341,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -381,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -487,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -629,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402B7E7-3202-0A4B-B9C7-989B3812537F}">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -986,7 +986,7 @@
         <v>29</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1585,7 +1585,7 @@
         <v>38</v>
       </c>
       <c r="B30">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>39</v>
@@ -1713,7 +1713,7 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>43</v>
@@ -2097,7 +2097,7 @@
         <v>54</v>
       </c>
       <c r="B46">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46">
         <v>52</v>
@@ -2129,7 +2129,7 @@
         <v>55</v>
       </c>
       <c r="B47">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C47">
         <v>53</v>
@@ -2321,7 +2321,7 @@
         <v>61</v>
       </c>
       <c r="B53">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C53">
         <v>58</v>
@@ -2737,7 +2737,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>73</v>
@@ -2769,7 +2769,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>73</v>
@@ -2868,7 +2868,7 @@
         <v>29</v>
       </c>
       <c r="C70">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D70">
         <v>0</v>

</xml_diff>

<commit_message>
g-tail confirmed working. Now to implement the others.
</commit_message>
<xml_diff>
--- a/misc/lookup_table.xlsx
+++ b/misc/lookup_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksidac/Documents/Programming/Undertale/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1201E0-3366-FA49-BA47-8FBA16CB87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43E2834-1215-8048-95DF-BD32B9EDBC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Letter</t>
   </si>
@@ -285,6 +285,21 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>q_union</t>
+  </si>
+  <si>
+    <t>p_union</t>
+  </si>
+  <si>
+    <t>g_union</t>
+  </si>
+  <si>
+    <t>Q_union</t>
+  </si>
+  <si>
+    <t>single_quote_union</t>
   </si>
 </sst>
 </file>
@@ -637,10 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402B7E7-3202-0A4B-B9C7-989B3812537F}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,9 +666,10 @@
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,8 +700,23 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -715,8 +747,11 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -747,8 +782,11 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -779,8 +817,11 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -811,8 +852,11 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -843,8 +887,11 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -875,8 +922,11 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -907,8 +957,11 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -939,8 +992,11 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -971,8 +1027,11 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1003,8 +1062,11 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1035,8 +1097,11 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1067,8 +1132,11 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1099,8 +1167,11 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1131,8 +1202,11 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1163,8 +1237,11 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1195,8 +1272,11 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1227,8 +1307,11 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1259,8 +1342,11 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1291,8 +1377,11 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1323,8 +1412,11 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1355,8 +1447,11 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1387,8 +1482,11 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1419,8 +1517,11 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1451,8 +1552,11 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1483,8 +1587,11 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1515,8 +1622,11 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1547,8 +1657,11 @@
       <c r="J28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1579,8 +1692,11 @@
       <c r="J29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1611,8 +1727,11 @@
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1643,8 +1762,11 @@
       <c r="J31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1675,8 +1797,11 @@
       <c r="J32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1707,8 +1832,11 @@
       <c r="J33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1739,8 +1867,11 @@
       <c r="J34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1771,8 +1902,11 @@
       <c r="J35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1803,8 +1937,11 @@
       <c r="J36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1835,8 +1972,11 @@
       <c r="J37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1867,8 +2007,11 @@
       <c r="J38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1899,8 +2042,11 @@
       <c r="J39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1931,8 +2077,11 @@
       <c r="J40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1963,8 +2112,11 @@
       <c r="J41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1995,8 +2147,11 @@
       <c r="J42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2027,8 +2182,11 @@
       <c r="J43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2059,8 +2217,11 @@
       <c r="J44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2091,8 +2252,11 @@
       <c r="J45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2123,8 +2287,11 @@
       <c r="J46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2155,8 +2322,11 @@
       <c r="J47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2187,8 +2357,11 @@
       <c r="J48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2219,8 +2392,11 @@
       <c r="J49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2251,8 +2427,11 @@
       <c r="J50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2283,8 +2462,11 @@
       <c r="J51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2315,8 +2497,11 @@
       <c r="J52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -2347,8 +2532,11 @@
       <c r="J53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>73</v>
       </c>
@@ -2379,8 +2567,11 @@
       <c r="J54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>74</v>
       </c>
@@ -2411,8 +2602,11 @@
       <c r="J55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
@@ -2443,8 +2637,11 @@
       <c r="J56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
@@ -2475,8 +2672,11 @@
       <c r="J57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -2507,8 +2707,11 @@
       <c r="J58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>78</v>
       </c>
@@ -2539,8 +2742,11 @@
       <c r="J59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
@@ -2571,8 +2777,11 @@
       <c r="J60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>79</v>
       </c>
@@ -2603,8 +2812,11 @@
       <c r="J61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>80</v>
       </c>
@@ -2635,8 +2847,11 @@
       <c r="J62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>81</v>
       </c>
@@ -2667,8 +2882,11 @@
       <c r="J63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2699,8 +2917,11 @@
       <c r="J64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2731,8 +2952,11 @@
       <c r="J65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2763,8 +2987,11 @@
       <c r="J66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2795,8 +3022,11 @@
       <c r="J67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2827,8 +3057,11 @@
       <c r="J68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2859,8 +3092,11 @@
       <c r="J69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2891,8 +3127,11 @@
       <c r="J70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="str">
         <f>CHAR(39)</f>
         <v>'</v>
@@ -2924,8 +3163,11 @@
       <c r="J71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -2956,8 +3198,11 @@
       <c r="J72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -2988,8 +3233,11 @@
       <c r="J73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -3020,8 +3268,11 @@
       <c r="J74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -3051,6 +3302,9 @@
       </c>
       <c r="J75">
         <v>0</v>
+      </c>
+      <c r="K75">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Q-tail. Now need to add comma-tail and we're all good
</commit_message>
<xml_diff>
--- a/misc/lookup_table.xlsx
+++ b/misc/lookup_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksidac/Documents/Programming/Undertale/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BF1161-AB48-304C-B8AD-4B3F41A89961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA924AC9-FC54-E24C-A842-21A59B644641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="27700" windowHeight="17500" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,8 +309,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -338,9 +346,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,9 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402B7E7-3202-0A4B-B9C7-989B3812537F}">
   <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,6 +771,9 @@
       <c r="M2">
         <v>30</v>
       </c>
+      <c r="N2">
+        <v>59</v>
+      </c>
       <c r="P2">
         <v>1</v>
       </c>
@@ -806,6 +818,9 @@
       <c r="M3">
         <v>96</v>
       </c>
+      <c r="N3">
+        <v>118</v>
+      </c>
       <c r="P3">
         <v>1</v>
       </c>
@@ -850,6 +865,9 @@
       <c r="M4">
         <v>30</v>
       </c>
+      <c r="N4">
+        <v>59</v>
+      </c>
       <c r="P4">
         <v>1</v>
       </c>
@@ -894,6 +912,9 @@
       <c r="M5">
         <v>95</v>
       </c>
+      <c r="N5">
+        <v>119</v>
+      </c>
       <c r="P5">
         <v>1</v>
       </c>
@@ -938,6 +959,9 @@
       <c r="M6">
         <v>30</v>
       </c>
+      <c r="N6">
+        <v>59</v>
+      </c>
       <c r="P6">
         <v>1</v>
       </c>
@@ -982,6 +1006,9 @@
       <c r="M7">
         <v>111</v>
       </c>
+      <c r="N7">
+        <v>120</v>
+      </c>
       <c r="P7">
         <v>0</v>
       </c>
@@ -1026,6 +1053,9 @@
       <c r="M8">
         <v>30</v>
       </c>
+      <c r="N8">
+        <v>59</v>
+      </c>
       <c r="P8">
         <v>1</v>
       </c>
@@ -1070,6 +1100,9 @@
       <c r="M9">
         <v>96</v>
       </c>
+      <c r="N9">
+        <v>118</v>
+      </c>
       <c r="P9">
         <v>1</v>
       </c>
@@ -1114,6 +1147,9 @@
       <c r="M10">
         <v>98</v>
       </c>
+      <c r="N10">
+        <v>121</v>
+      </c>
       <c r="P10">
         <v>1</v>
       </c>
@@ -1158,6 +1194,9 @@
       <c r="M11">
         <v>95</v>
       </c>
+      <c r="N11">
+        <v>119</v>
+      </c>
       <c r="P11">
         <v>1</v>
       </c>
@@ -1202,6 +1241,9 @@
       <c r="M12">
         <v>96</v>
       </c>
+      <c r="N12">
+        <v>118</v>
+      </c>
       <c r="P12">
         <v>1</v>
       </c>
@@ -1246,6 +1288,9 @@
       <c r="M13">
         <v>104</v>
       </c>
+      <c r="N13">
+        <v>122</v>
+      </c>
       <c r="P13">
         <v>1</v>
       </c>
@@ -1290,6 +1335,9 @@
       <c r="M14">
         <v>30</v>
       </c>
+      <c r="N14">
+        <v>59</v>
+      </c>
       <c r="P14">
         <v>1</v>
       </c>
@@ -1334,6 +1382,9 @@
       <c r="M15">
         <v>30</v>
       </c>
+      <c r="N15">
+        <v>59</v>
+      </c>
       <c r="P15">
         <v>1</v>
       </c>
@@ -1378,6 +1429,9 @@
       <c r="M16">
         <v>30</v>
       </c>
+      <c r="N16">
+        <v>59</v>
+      </c>
       <c r="P16">
         <v>1</v>
       </c>
@@ -1422,6 +1476,9 @@
       <c r="M17">
         <v>30</v>
       </c>
+      <c r="N17">
+        <v>59</v>
+      </c>
       <c r="P17">
         <v>1</v>
       </c>
@@ -1466,6 +1523,9 @@
       <c r="M18">
         <v>30</v>
       </c>
+      <c r="N18">
+        <v>59</v>
+      </c>
       <c r="P18">
         <v>1</v>
       </c>
@@ -1510,6 +1570,9 @@
       <c r="M19">
         <v>30</v>
       </c>
+      <c r="N19">
+        <v>59</v>
+      </c>
       <c r="P19">
         <v>1</v>
       </c>
@@ -1554,6 +1617,9 @@
       <c r="M20">
         <v>30</v>
       </c>
+      <c r="N20">
+        <v>59</v>
+      </c>
       <c r="P20">
         <v>1</v>
       </c>
@@ -1598,6 +1664,9 @@
       <c r="M21">
         <v>98</v>
       </c>
+      <c r="N21">
+        <v>121</v>
+      </c>
       <c r="P21">
         <v>1</v>
       </c>
@@ -1642,6 +1711,9 @@
       <c r="M22">
         <v>30</v>
       </c>
+      <c r="N22">
+        <v>59</v>
+      </c>
       <c r="P22">
         <v>1</v>
       </c>
@@ -1686,6 +1758,9 @@
       <c r="M23">
         <v>30</v>
       </c>
+      <c r="N23">
+        <v>59</v>
+      </c>
       <c r="P23">
         <v>1</v>
       </c>
@@ -1730,6 +1805,9 @@
       <c r="M24">
         <v>30</v>
       </c>
+      <c r="N24">
+        <v>59</v>
+      </c>
       <c r="P24">
         <v>1</v>
       </c>
@@ -1774,6 +1852,9 @@
       <c r="M25">
         <v>30</v>
       </c>
+      <c r="N25">
+        <v>59</v>
+      </c>
       <c r="P25">
         <v>1</v>
       </c>
@@ -1817,6 +1898,9 @@
       </c>
       <c r="M26">
         <v>30</v>
+      </c>
+      <c r="N26">
+        <v>59</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -1862,6 +1946,9 @@
       <c r="M27">
         <v>30</v>
       </c>
+      <c r="N27">
+        <v>59</v>
+      </c>
       <c r="P27">
         <v>1</v>
       </c>
@@ -1906,6 +1993,9 @@
       <c r="M28">
         <v>100</v>
       </c>
+      <c r="N28">
+        <v>123</v>
+      </c>
       <c r="P28">
         <v>1</v>
       </c>
@@ -1950,6 +2040,9 @@
       <c r="M29">
         <v>112</v>
       </c>
+      <c r="N29">
+        <v>124</v>
+      </c>
       <c r="P29">
         <v>0</v>
       </c>
@@ -1994,6 +2087,9 @@
       <c r="M30">
         <v>100</v>
       </c>
+      <c r="N30">
+        <v>123</v>
+      </c>
       <c r="P30">
         <v>1</v>
       </c>
@@ -2038,6 +2134,9 @@
       <c r="M31">
         <v>112</v>
       </c>
+      <c r="N31">
+        <v>124</v>
+      </c>
       <c r="P31">
         <v>0</v>
       </c>
@@ -2082,6 +2181,9 @@
       <c r="M32">
         <v>102</v>
       </c>
+      <c r="N32">
+        <v>125</v>
+      </c>
       <c r="P32">
         <v>1</v>
       </c>
@@ -2126,6 +2228,9 @@
       <c r="M33">
         <v>102</v>
       </c>
+      <c r="N33">
+        <v>125</v>
+      </c>
       <c r="P33">
         <v>1</v>
       </c>
@@ -2170,6 +2275,9 @@
       <c r="M34">
         <v>100</v>
       </c>
+      <c r="N34">
+        <v>123</v>
+      </c>
       <c r="P34">
         <v>1</v>
       </c>
@@ -2214,6 +2322,9 @@
       <c r="M35">
         <v>103</v>
       </c>
+      <c r="N35">
+        <v>126</v>
+      </c>
       <c r="P35">
         <v>1</v>
       </c>
@@ -2258,6 +2369,9 @@
       <c r="M36">
         <v>102</v>
       </c>
+      <c r="N36">
+        <v>125</v>
+      </c>
       <c r="P36">
         <v>1</v>
       </c>
@@ -2302,6 +2416,9 @@
       <c r="M37">
         <v>99</v>
       </c>
+      <c r="N37">
+        <v>127</v>
+      </c>
       <c r="P37">
         <v>1</v>
       </c>
@@ -2346,6 +2463,9 @@
       <c r="M38">
         <v>103</v>
       </c>
+      <c r="N38">
+        <v>126</v>
+      </c>
       <c r="P38">
         <v>1</v>
       </c>
@@ -2390,6 +2510,9 @@
       <c r="M39">
         <v>96</v>
       </c>
+      <c r="N39">
+        <v>118</v>
+      </c>
       <c r="P39">
         <v>1</v>
       </c>
@@ -2434,6 +2557,9 @@
       <c r="M40">
         <v>113</v>
       </c>
+      <c r="N40">
+        <v>128</v>
+      </c>
       <c r="P40">
         <v>0</v>
       </c>
@@ -2478,6 +2604,9 @@
       <c r="M41">
         <v>103</v>
       </c>
+      <c r="N41">
+        <v>126</v>
+      </c>
       <c r="P41">
         <v>1</v>
       </c>
@@ -2522,6 +2651,9 @@
       <c r="M42">
         <v>100</v>
       </c>
+      <c r="N42">
+        <v>123</v>
+      </c>
       <c r="P42">
         <v>1</v>
       </c>
@@ -2566,6 +2698,9 @@
       <c r="M43">
         <v>112</v>
       </c>
+      <c r="N43">
+        <v>124</v>
+      </c>
       <c r="P43">
         <v>0</v>
       </c>
@@ -2610,6 +2745,9 @@
       <c r="M44">
         <v>100</v>
       </c>
+      <c r="N44">
+        <v>123</v>
+      </c>
       <c r="P44">
         <v>1</v>
       </c>
@@ -2654,6 +2792,9 @@
       <c r="M45">
         <v>112</v>
       </c>
+      <c r="N45">
+        <v>124</v>
+      </c>
       <c r="P45">
         <v>0</v>
       </c>
@@ -2698,6 +2839,9 @@
       <c r="M46">
         <v>100</v>
       </c>
+      <c r="N46">
+        <v>123</v>
+      </c>
       <c r="P46">
         <v>1</v>
       </c>
@@ -2742,6 +2886,9 @@
       <c r="M47">
         <v>102</v>
       </c>
+      <c r="N47">
+        <v>125</v>
+      </c>
       <c r="P47">
         <v>1</v>
       </c>
@@ -2786,6 +2933,9 @@
       <c r="M48">
         <v>103</v>
       </c>
+      <c r="N48">
+        <v>126</v>
+      </c>
       <c r="P48">
         <v>1</v>
       </c>
@@ -2830,6 +2980,9 @@
       <c r="M49">
         <v>103</v>
       </c>
+      <c r="N49">
+        <v>126</v>
+      </c>
       <c r="P49">
         <v>1</v>
       </c>
@@ -2874,6 +3027,9 @@
       <c r="M50">
         <v>114</v>
       </c>
+      <c r="N50">
+        <v>129</v>
+      </c>
       <c r="P50">
         <v>0</v>
       </c>
@@ -2918,6 +3074,9 @@
       <c r="M51">
         <v>103</v>
       </c>
+      <c r="N51">
+        <v>126</v>
+      </c>
       <c r="P51">
         <v>1</v>
       </c>
@@ -2962,6 +3121,9 @@
       <c r="M52">
         <v>103</v>
       </c>
+      <c r="N52">
+        <v>126</v>
+      </c>
       <c r="P52">
         <v>1</v>
       </c>
@@ -3006,6 +3168,9 @@
       <c r="M53">
         <v>102</v>
       </c>
+      <c r="N53">
+        <v>125</v>
+      </c>
       <c r="P53">
         <v>1</v>
       </c>
@@ -3050,6 +3215,9 @@
       <c r="M54">
         <v>100</v>
       </c>
+      <c r="N54">
+        <v>123</v>
+      </c>
       <c r="P54">
         <v>1</v>
       </c>
@@ -3094,6 +3262,9 @@
       <c r="M55">
         <v>98</v>
       </c>
+      <c r="N55">
+        <v>121</v>
+      </c>
       <c r="P55">
         <v>1</v>
       </c>
@@ -3138,6 +3309,9 @@
       <c r="M56">
         <v>100</v>
       </c>
+      <c r="N56">
+        <v>123</v>
+      </c>
       <c r="P56">
         <v>1</v>
       </c>
@@ -3182,6 +3356,9 @@
       <c r="M57">
         <v>100</v>
       </c>
+      <c r="N57">
+        <v>123</v>
+      </c>
       <c r="P57">
         <v>1</v>
       </c>
@@ -3226,6 +3403,9 @@
       <c r="M58">
         <v>95</v>
       </c>
+      <c r="N58">
+        <v>119</v>
+      </c>
       <c r="P58">
         <v>1</v>
       </c>
@@ -3270,6 +3450,9 @@
       <c r="M59">
         <v>102</v>
       </c>
+      <c r="N59">
+        <v>125</v>
+      </c>
       <c r="P59">
         <v>1</v>
       </c>
@@ -3314,6 +3497,9 @@
       <c r="M60">
         <v>99</v>
       </c>
+      <c r="N60">
+        <v>127</v>
+      </c>
       <c r="P60">
         <v>1</v>
       </c>
@@ -3358,6 +3544,9 @@
       <c r="M61">
         <v>102</v>
       </c>
+      <c r="N61">
+        <v>125</v>
+      </c>
       <c r="P61">
         <v>1</v>
       </c>
@@ -3402,6 +3591,9 @@
       <c r="M62">
         <v>100</v>
       </c>
+      <c r="N62">
+        <v>123</v>
+      </c>
       <c r="P62">
         <v>1</v>
       </c>
@@ -3446,6 +3638,9 @@
       <c r="M63">
         <v>100</v>
       </c>
+      <c r="N63">
+        <v>123</v>
+      </c>
       <c r="P63">
         <v>1</v>
       </c>
@@ -3490,6 +3685,9 @@
       <c r="M64">
         <v>30</v>
       </c>
+      <c r="N64">
+        <v>59</v>
+      </c>
       <c r="P64">
         <v>1</v>
       </c>
@@ -3534,6 +3732,9 @@
       <c r="M65">
         <v>30</v>
       </c>
+      <c r="N65" s="2">
+        <v>59</v>
+      </c>
       <c r="P65">
         <v>1</v>
       </c>
@@ -3578,6 +3779,9 @@
       <c r="M66">
         <v>98</v>
       </c>
+      <c r="N66">
+        <v>121</v>
+      </c>
       <c r="P66">
         <v>1</v>
       </c>
@@ -3622,6 +3826,9 @@
       <c r="M67">
         <v>98</v>
       </c>
+      <c r="N67">
+        <v>121</v>
+      </c>
       <c r="P67">
         <v>1</v>
       </c>
@@ -3666,6 +3873,9 @@
       <c r="M68">
         <v>30</v>
       </c>
+      <c r="N68">
+        <v>59</v>
+      </c>
       <c r="P68">
         <v>1</v>
       </c>
@@ -3710,6 +3920,9 @@
       <c r="M69">
         <v>115</v>
       </c>
+      <c r="N69">
+        <v>130</v>
+      </c>
       <c r="P69">
         <v>0</v>
       </c>
@@ -3753,6 +3966,9 @@
       </c>
       <c r="M70">
         <v>108</v>
+      </c>
+      <c r="N70">
+        <v>131</v>
       </c>
       <c r="P70">
         <v>1</v>
@@ -3799,6 +4015,9 @@
       <c r="M71">
         <v>116</v>
       </c>
+      <c r="N71">
+        <v>132</v>
+      </c>
       <c r="P71">
         <v>0</v>
       </c>
@@ -3843,6 +4062,9 @@
       <c r="M72">
         <v>117</v>
       </c>
+      <c r="N72">
+        <v>133</v>
+      </c>
       <c r="P72">
         <v>0</v>
       </c>
@@ -3887,6 +4109,9 @@
       <c r="M73">
         <v>30</v>
       </c>
+      <c r="N73">
+        <v>59</v>
+      </c>
       <c r="P73">
         <v>1</v>
       </c>
@@ -3931,6 +4156,9 @@
       <c r="M74">
         <v>104</v>
       </c>
+      <c r="N74">
+        <v>122</v>
+      </c>
       <c r="P74">
         <v>1</v>
       </c>
@@ -3974,6 +4202,9 @@
       </c>
       <c r="M75">
         <v>99</v>
+      </c>
+      <c r="N75">
+        <v>127</v>
       </c>
       <c r="P75">
         <v>1</v>

</xml_diff>

<commit_message>
Finished it. Going to get lunch. Will comment it heavily afterwards
</commit_message>
<xml_diff>
--- a/misc/lookup_table.xlsx
+++ b/misc/lookup_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksidac/Documents/Programming/Undertale/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA0C305-6D08-2B44-86AA-F9E1B94B22CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E036095-A619-F043-AFC7-A96A0BC97872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="500" windowWidth="27700" windowHeight="17500" xr2:uid="{B507ECB4-3C8B-AE46-8143-D44287263394}"/>
   </bookViews>
@@ -666,9 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402B7E7-3202-0A4B-B9C7-989B3812537F}">
   <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O58" sqref="O58"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2:P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>